<commit_message>
Correct typo in site distance matrix
</commit_message>
<xml_diff>
--- a/2020/distance.xlsx
+++ b/2020/distance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhundt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4d8ee2329758792/Documents/SESYNC/Carp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1E0796-C6E0-2E45-8D94-B8A2D2ED7C4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AFBF656-58C2-441D-86F2-A76BCC5660FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="960" windowWidth="28040" windowHeight="16940" xr2:uid="{338C1FC5-2BCE-6D46-9CF6-4E3AE3B07D75}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{338C1FC5-2BCE-6D46-9CF6-4E3AE3B07D75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,12 +391,12 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -422,7 +422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -451,7 +451,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -480,7 +480,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,7 +509,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -538,7 +538,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -564,10 +564,10 @@
         <v>1132</v>
       </c>
       <c r="I6">
-        <v>11767</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -596,7 +596,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -625,7 +625,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>

</xml_diff>